<commit_message>
update week 4 quiz questions
</commit_message>
<xml_diff>
--- a/materials/Week4Questions.xlsx
+++ b/materials/Week4Questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cimac\OneDrive\Documents\GitHub\statistics\materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cimacint\Documents\GitHub\statistics\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{C61F9A18-7907-4E84-90F6-211130C500C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0A7E6361-9A0A-4ECC-83E4-856D2F2E729A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087238E5-D3AC-4F83-A985-603DEF90218E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1608" yWindow="264" windowWidth="19572" windowHeight="11724" xr2:uid="{F51AF9FE-1576-4C0C-B963-4870BE35EA56}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{F51AF9FE-1576-4C0C-B963-4870BE35EA56}"/>
   </bookViews>
   <sheets>
     <sheet name="Quiz" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="406">
   <si>
     <t>https://www.youtube.com/watch?v=1PsPfMaLWSk</t>
   </si>
@@ -1202,7 +1202,52 @@
     <t>Old questions kept for examples.</t>
   </si>
   <si>
-    <t>Null hypothesis significance testing</t>
+    <t>w04001</t>
+  </si>
+  <si>
+    <t>Statistical Hypothesis Inference Testing is another name for Null Hypothesis Significance Testing.</t>
+  </si>
+  <si>
+    <t>Field 3.2</t>
+  </si>
+  <si>
+    <t>In NHST a statistically significant result means that the effect is clinically important.</t>
+  </si>
+  <si>
+    <t>In NHST a non-significant result means the null hypothesis is true.</t>
+  </si>
+  <si>
+    <t>In NHST a non-significant result means the effect was not large enough to be detected given the sample size.</t>
+  </si>
+  <si>
+    <t>In NHST a statistically significant result means the null hypothesis is false.</t>
+  </si>
+  <si>
+    <t>One problem with NHST is it encourages all or nothing thinking.</t>
+  </si>
+  <si>
+    <t>A statistical test with a p-value of 0.0501 and another with a p-value of 0.0499 would likely have about the same effect size.</t>
+  </si>
+  <si>
+    <t>The conclusions from NHST are dependent on the intentions of the scientist before data are collected.</t>
+  </si>
+  <si>
+    <t>Type I (alpha) and Type II (beta) error rates are probabilities expected from repeated identical experiments (long-run probabilities).</t>
+  </si>
+  <si>
+    <t>Researcher degrees of freedom' refers to the fact that researchers have many decisions to make when designing and analyzing a study.</t>
+  </si>
+  <si>
+    <t>p-hacking is selective reporting of significant results.</t>
+  </si>
+  <si>
+    <t>HARKing is hypothesizing after the results are known.</t>
+  </si>
+  <si>
+    <t>p-hacking and HARKing are ways to cheat the NHST system.</t>
+  </si>
+  <si>
+    <t>p-hacking and HARKing increase the Type 1 error rate.</t>
   </si>
 </sst>
 </file>
@@ -1558,19 +1603,19 @@
   <dimension ref="A1:AH156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="17" max="17" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>347</v>
       </c>
@@ -1674,17 +1719,136 @@
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="D2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>394</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>395</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>396</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>397</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>398</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>400</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D11" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>402</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>403</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>404</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>405</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>381</v>
       </c>
@@ -1704,7 +1868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>381</v>
       </c>
@@ -1724,7 +1888,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>381</v>
       </c>
@@ -1744,7 +1908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>381</v>
       </c>
@@ -1764,7 +1928,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>381</v>
       </c>
@@ -1784,7 +1948,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>381</v>
       </c>
@@ -1804,7 +1968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>381</v>
       </c>
@@ -1824,7 +1988,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>382</v>
       </c>
@@ -1856,7 +2020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>381</v>
       </c>
@@ -1876,7 +2040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>381</v>
       </c>
@@ -1896,7 +2060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>381</v>
       </c>
@@ -1916,7 +2080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>381</v>
       </c>
@@ -1936,7 +2100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>381</v>
       </c>
@@ -1956,7 +2120,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>381</v>
       </c>
@@ -1976,7 +2140,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>381</v>
       </c>
@@ -1996,7 +2160,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>381</v>
       </c>
@@ -2016,7 +2180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>381</v>
       </c>
@@ -2036,7 +2200,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>381</v>
       </c>
@@ -2056,7 +2220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>381</v>
       </c>
@@ -2076,7 +2240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>381</v>
       </c>
@@ -2096,7 +2260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>382</v>
       </c>
@@ -2131,7 +2295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>381</v>
       </c>
@@ -2151,7 +2315,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>381</v>
       </c>
@@ -2171,7 +2335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>382</v>
       </c>
@@ -2206,7 +2370,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>381</v>
       </c>
@@ -2226,7 +2390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>381</v>
       </c>
@@ -2246,7 +2410,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>381</v>
       </c>
@@ -2266,7 +2430,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>381</v>
       </c>
@@ -2286,7 +2450,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>381</v>
       </c>
@@ -2306,7 +2470,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>381</v>
       </c>
@@ -2326,7 +2490,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>381</v>
       </c>
@@ -2346,7 +2510,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>381</v>
       </c>
@@ -2366,7 +2530,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>381</v>
       </c>
@@ -2386,7 +2550,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>383</v>
       </c>
@@ -2436,7 +2600,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>383</v>
       </c>
@@ -2486,7 +2650,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>383</v>
       </c>
@@ -2518,7 +2682,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>383</v>
       </c>
@@ -2556,7 +2720,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>381</v>
       </c>
@@ -2576,7 +2740,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>381</v>
       </c>
@@ -2596,7 +2760,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>381</v>
       </c>
@@ -2616,7 +2780,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>381</v>
       </c>
@@ -2636,7 +2800,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>381</v>
       </c>
@@ -2656,7 +2820,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>381</v>
       </c>
@@ -2676,7 +2840,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>382</v>
       </c>
@@ -2705,7 +2869,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>382</v>
       </c>
@@ -2734,7 +2898,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>382</v>
       </c>
@@ -2763,7 +2927,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>382</v>
       </c>
@@ -2792,7 +2956,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>382</v>
       </c>
@@ -2821,7 +2985,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>382</v>
       </c>
@@ -2850,7 +3014,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>382</v>
       </c>
@@ -2879,7 +3043,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>382</v>
       </c>
@@ -2908,7 +3072,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>382</v>
       </c>
@@ -2937,7 +3101,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>382</v>
       </c>
@@ -2966,7 +3130,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>382</v>
       </c>
@@ -2995,7 +3159,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>383</v>
       </c>
@@ -3045,7 +3209,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>383</v>
       </c>
@@ -3092,7 +3256,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>383</v>
       </c>
@@ -3130,7 +3294,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>383</v>
       </c>
@@ -3168,7 +3332,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>383</v>
       </c>
@@ -3218,7 +3382,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>383</v>
       </c>
@@ -3268,7 +3432,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>383</v>
       </c>
@@ -3318,7 +3482,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>383</v>
       </c>
@@ -3368,7 +3532,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>381</v>
       </c>
@@ -3388,7 +3552,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>381</v>
       </c>
@@ -3408,7 +3572,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>382</v>
       </c>
@@ -3443,7 +3607,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>382</v>
       </c>
@@ -3478,7 +3642,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>382</v>
       </c>
@@ -3513,7 +3677,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>382</v>
       </c>
@@ -3548,7 +3712,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>381</v>
       </c>
@@ -3568,7 +3732,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>381</v>
       </c>
@@ -3588,7 +3752,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>381</v>
       </c>
@@ -3608,7 +3772,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>381</v>
       </c>
@@ -3628,7 +3792,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>381</v>
       </c>
@@ -3648,7 +3812,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>381</v>
       </c>
@@ -3668,7 +3832,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>381</v>
       </c>
@@ -3688,7 +3852,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>381</v>
       </c>
@@ -3708,7 +3872,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>381</v>
       </c>
@@ -3728,7 +3892,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>381</v>
       </c>
@@ -3748,7 +3912,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>381</v>
       </c>
@@ -3768,7 +3932,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>381</v>
       </c>
@@ -3788,7 +3952,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>381</v>
       </c>
@@ -3808,7 +3972,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>381</v>
       </c>
@@ -3828,7 +3992,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>381</v>
       </c>
@@ -3848,7 +4012,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -3868,7 +4032,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>381</v>
       </c>
@@ -3888,7 +4052,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>381</v>
       </c>
@@ -3908,7 +4072,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>381</v>
       </c>
@@ -3928,7 +4092,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>381</v>
       </c>
@@ -3948,7 +4112,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>381</v>
       </c>
@@ -3968,7 +4132,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>381</v>
       </c>
@@ -3988,7 +4152,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>381</v>
       </c>
@@ -4008,7 +4172,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>381</v>
       </c>
@@ -4028,7 +4192,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>381</v>
       </c>
@@ -4048,7 +4212,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>381</v>
       </c>
@@ -4068,7 +4232,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>382</v>
       </c>
@@ -4103,7 +4267,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>382</v>
       </c>
@@ -4138,7 +4302,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>382</v>
       </c>
@@ -4173,7 +4337,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>382</v>
       </c>
@@ -4208,7 +4372,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>382</v>
       </c>
@@ -4243,7 +4407,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>382</v>
       </c>
@@ -4278,7 +4442,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>382</v>
       </c>
@@ -4313,7 +4477,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>382</v>
       </c>
@@ -4348,7 +4512,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>382</v>
       </c>
@@ -4383,7 +4547,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>382</v>
       </c>
@@ -4418,7 +4582,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>382</v>
       </c>
@@ -4453,7 +4617,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>382</v>
       </c>
@@ -4488,7 +4652,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>382</v>
       </c>
@@ -4523,7 +4687,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>382</v>
       </c>
@@ -4558,7 +4722,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>382</v>
       </c>
@@ -4593,7 +4757,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>382</v>
       </c>
@@ -4628,7 +4792,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>382</v>
       </c>
@@ -4663,7 +4827,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>382</v>
       </c>
@@ -4698,7 +4862,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>382</v>
       </c>
@@ -4733,7 +4897,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>382</v>
       </c>
@@ -4768,7 +4932,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>382</v>
       </c>
@@ -4803,7 +4967,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>382</v>
       </c>
@@ -4838,7 +5002,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>382</v>
       </c>
@@ -4873,7 +5037,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>382</v>
       </c>
@@ -4908,7 +5072,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>382</v>
       </c>
@@ -4943,7 +5107,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>382</v>
       </c>
@@ -4978,7 +5142,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>382</v>
       </c>
@@ -5013,7 +5177,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>382</v>
       </c>
@@ -5048,7 +5212,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>382</v>
       </c>
@@ -5083,7 +5247,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>382</v>
       </c>
@@ -5118,7 +5282,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>382</v>
       </c>
@@ -5153,7 +5317,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>382</v>
       </c>

</xml_diff>